<commit_message>
Gera últimos gráficso para relatório PIBITI CNPq
</commit_message>
<xml_diff>
--- a/ESTADOSP/Parameters_São José dos Campos.xlsx
+++ b/ESTADOSP/Parameters_São José dos Campos.xlsx
@@ -468,16 +468,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>5697</v>
+        <v>12262</v>
       </c>
       <c r="D2" t="n">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="E2" t="n">
-        <v>2.192</v>
+        <v>0.593</v>
       </c>
       <c r="F2" t="n">
-        <v>10.2</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="3">
@@ -488,16 +488,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>14922</v>
+        <v>8979</v>
       </c>
       <c r="D3" t="n">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E3" t="n">
         <v>0.1</v>
       </c>
       <c r="F3" t="n">
-        <v>26.7</v>
+        <v>31.2</v>
       </c>
     </row>
     <row r="4">
@@ -508,16 +508,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>28920</v>
+        <v>29466</v>
       </c>
       <c r="D4" t="n">
         <v>332</v>
       </c>
       <c r="E4" t="n">
-        <v>0.903</v>
+        <v>0.572</v>
       </c>
       <c r="F4" t="n">
-        <v>15.8</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="5">
@@ -528,16 +528,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>43114</v>
+        <v>42975</v>
       </c>
       <c r="D5" t="n">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F5" t="n">
-        <v>29.4</v>
+        <v>42.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>